<commit_message>
added phpExcel libray for import in lead search management
</commit_message>
<xml_diff>
--- a/uploads/test.xlsx
+++ b/uploads/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\crm-new\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD6A5A6-B0BA-4DEA-A331-D045F109FCB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFCA1D3-9AB7-4149-8894-644ADE1BDED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
   <si>
     <t>Kids Dresses</t>
   </si>
@@ -42,21 +42,12 @@
     <t>Email</t>
   </si>
   <si>
-    <t>afsar@gmail.com</t>
-  </si>
-  <si>
-    <t>afsar1@gmail.com</t>
-  </si>
-  <si>
     <t>afs222ar@gmail.com</t>
   </si>
   <si>
     <t>a2222222222fsar@gmail.com</t>
   </si>
   <si>
-    <t>afs2312222222ar1@gmail.com</t>
-  </si>
-  <si>
     <t>saquibrah321mani007@gmail.com</t>
   </si>
   <si>
@@ -169,6 +160,12 @@
   </si>
   <si>
     <t>geasdfasdfddfsar@gmail.com</t>
+  </si>
+  <si>
+    <t>afs231443453453453453452222222ar1@gmail.com</t>
+  </si>
+  <si>
+    <t>eqewwewrq@dsa.com</t>
   </si>
 </sst>
 </file>
@@ -557,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,76 +578,76 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" t="s">
-        <v>34</v>
-      </c>
-      <c r="T1" t="s">
-        <v>35</v>
-      </c>
-      <c r="U1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" t="s">
-        <v>37</v>
-      </c>
-      <c r="W1" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -664,15 +661,15 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E2">
-        <v>2123234</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -680,9 +677,7 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -695,10 +690,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>37901</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -712,7 +704,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>234000234</v>
@@ -729,10 +721,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="E6">
-        <v>3569342234</v>
+        <v>3532342369342230</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -746,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>5324</v>
@@ -763,7 +755,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8">
         <v>9421269234</v>
@@ -780,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <v>6963744234</v>
@@ -797,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>85379</v>
@@ -805,7 +797,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -814,7 +806,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>33383452</v>
@@ -823,16 +815,16 @@
         <v>342</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I11">
         <v>345344</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K11">
         <v>435345</v>
@@ -841,28 +833,28 @@
         <v>3</v>
       </c>
       <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" t="s">
+        <v>42</v>
+      </c>
+      <c r="P11" t="s">
         <v>43</v>
       </c>
-      <c r="N11" t="s">
+      <c r="Q11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T11" t="s">
         <v>44</v>
-      </c>
-      <c r="O11" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>46</v>
-      </c>
-      <c r="R11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S11" t="s">
-        <v>46</v>
-      </c>
-      <c r="T11" t="s">
-        <v>47</v>
       </c>
       <c r="U11">
         <v>2</v>
@@ -880,18 +872,17 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{9DAE5BC1-094A-4E17-BAE4-AE7BAC86A92F}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{E1AD813F-B3A5-4116-BF36-26841A0ACE9F}"/>
-    <hyperlink ref="D6" r:id="rId3" xr:uid="{F50D5A15-B72C-4458-BC17-E03705A56EC3}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{8FAA2DCD-A603-465E-9D0D-83B4FEA81092}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{6B441214-FD2B-45C2-91B3-FC5F46342097}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{0B76F6EB-AC57-471F-AD59-BBC2325AF322}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{F9A51474-A146-4578-9154-CAEBA2F9669E}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{5B1B580A-CE18-4FF8-BF51-E44C6EFD09F9}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{4104646D-86BE-4B15-B5A7-0C038949066A}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{23772C6A-E6DB-48F1-921A-F24911100C65}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{F50D5A15-B72C-4458-BC17-E03705A56EC3}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{8FAA2DCD-A603-465E-9D0D-83B4FEA81092}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{6B441214-FD2B-45C2-91B3-FC5F46342097}"/>
+    <hyperlink ref="D9" r:id="rId5" xr:uid="{F9A51474-A146-4578-9154-CAEBA2F9669E}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{5B1B580A-CE18-4FF8-BF51-E44C6EFD09F9}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{4104646D-86BE-4B15-B5A7-0C038949066A}"/>
+    <hyperlink ref="D11" r:id="rId8" xr:uid="{23772C6A-E6DB-48F1-921A-F24911100C65}"/>
+    <hyperlink ref="D2" r:id="rId9" xr:uid="{1B9E7D2B-0B9A-41CC-A7B0-74C4AC7D7DD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>